<commit_message>
make it lesson to private messages
</commit_message>
<xml_diff>
--- a/core/guild.xlsx
+++ b/core/guild.xlsx
@@ -15,13 +15,90 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <si>
+    <t>1076954067823251617</t>
+  </si>
+  <si>
+    <t>1079112886967873606</t>
+  </si>
+  <si>
+    <t>Badge_bot_server</t>
+  </si>
+  <si>
+    <t>live</t>
+  </si>
+  <si>
+    <t>1091933458525327513</t>
+  </si>
+  <si>
+    <t>1091933459192238162</t>
+  </si>
+  <si>
+    <t>kyoharo's server</t>
+  </si>
+  <si>
+    <t>general</t>
+  </si>
+  <si>
+    <t>1091961825781891163</t>
+  </si>
+  <si>
+    <t>1121082544377569410</t>
+  </si>
+  <si>
+    <t>kyoharo</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>1114187435497246891</t>
+  </si>
+  <si>
+    <t>1114187435497246894</t>
+  </si>
+  <si>
+    <t>AVCB Team</t>
+  </si>
+  <si>
+    <t>avc-bot</t>
+  </si>
+  <si>
+    <t>987051677045624912</t>
+  </si>
+  <si>
+    <t>1079836876506153093</t>
+  </si>
+  <si>
+    <t>W45</t>
+  </si>
+  <si>
+    <t>⑇المـسـاعد-الخـفي</t>
+  </si>
+  <si>
+    <t>1002704246287900792</t>
+  </si>
+  <si>
+    <t>1110359019845070918</t>
+  </si>
+  <si>
+    <t>狐. - 𝑲𝑰𝑻𝑺𝑼𝑵𝑬.</t>
+  </si>
+  <si>
+    <t>𝑪𝒉𝒂𝒕𝑩𝒐𝒕-🤖-ذكاء-صناعي</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -32,46 +109,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -93,6 +149,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -101,31 +164,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -139,6 +194,51 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -147,30 +247,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -191,43 +268,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -239,72 +430,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -317,65 +442,41 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -418,15 +519,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -444,9 +536,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -468,11 +562,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -481,154 +573,160 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="6">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="7">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="3">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="8">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="5">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -978,14 +1076,105 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A2:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="C8" sqref="A8:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="21.3333333333333" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.3333333333333" customWidth="1"/>
+    <col min="3" max="3" width="28.7777777777778" customWidth="1"/>
+    <col min="4" max="4" width="36.9259259259259" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>

</xml_diff>